<commit_message>
ExcelReader no longer raises IndexError and check date vs datetime object
</commit_message>
<xml_diff>
--- a/tests/samples/excel_datatypes.xlsx
+++ b/tests/samples/excel_datatypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.borbely\code\git\msl-io\tests\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\photon\code\msl-io\tests\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C82646-6FB0-48E1-BC20-1B3BFB82B34F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4189BA41-65A1-4143-8277-9003B8EE8A8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3893" yWindow="2062" windowWidth="14145" windowHeight="11018" xr2:uid="{F5C99075-6A6F-4D35-9698-7A4B546F45AE}"/>
+    <workbookView xWindow="-24945" yWindow="3330" windowWidth="21600" windowHeight="11385" xr2:uid="{F5C99075-6A6F-4D35-9698-7A4B546F45AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +46,14 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,19 +79,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,18 +407,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFBC155-3483-46AB-B243-BB2650B87F12}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
         <v>1.23</v>
       </c>
@@ -414,14 +429,20 @@
       <c r="C1" s="1">
         <v>43721.555806828706</v>
       </c>
+      <c r="D1" s="4">
+        <v>43721</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>PI()</f>
         <v>3.1415926535897931</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>